<commit_message>
Actualice README.md para aclarar el impacto de las transformaciones en las figuras de la imagen; modifique resultados_romboide.xlsx para obtener resultados de análisis actualizados.
</commit_message>
<xml_diff>
--- a/resultados_romboide.xlsx
+++ b/resultados_romboide.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,15 +436,20 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Carpeta</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Imagen</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Área</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Perímetro</t>
         </is>
@@ -453,261 +458,541 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>romboide-and.jpg</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>33004</v>
+          <t>filtros</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>romboide-desenfocado-blur.jpg</t>
+        </is>
       </c>
       <c r="C2" t="n">
+        <v>33004</v>
+      </c>
+      <c r="D2" t="n">
         <v>742</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>romboide-binarizado.jpg</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>33004</v>
+          <t>filtros</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>romboide-desenfocado-Gaussiano.jpg</t>
+        </is>
       </c>
       <c r="C3" t="n">
+        <v>33004</v>
+      </c>
+      <c r="D3" t="n">
         <v>742</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>romboide-desenfocado-blur.jpg</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>33004</v>
+          <t>filtros</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>romboide-nitidez.jpg</t>
+        </is>
       </c>
       <c r="C4" t="n">
-        <v>742</v>
+        <v>32870</v>
+      </c>
+      <c r="D4" t="n">
+        <v>844.4995617866516</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>romboide-desenfocado-Gaussiano.jpg</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>33004</v>
+          <t>filtros</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>romboide_bordes.jpg</t>
+        </is>
       </c>
       <c r="C5" t="n">
-        <v>742</v>
+        <v>8967.5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>411.3797236680984</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>romboide-division.jpg</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
+          <t>filtros</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>romboide_dilatado.jpg</t>
+        </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>33004</v>
+      </c>
+      <c r="D6" t="n">
+        <v>742</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>romboide-gris.jpg</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>33004</v>
+          <t>filtros</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>romboide_Relieve.jpg</t>
+        </is>
       </c>
       <c r="C7" t="n">
-        <v>742</v>
+        <v>33001</v>
+      </c>
+      <c r="D7" t="n">
+        <v>744.4852812290192</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>romboide-interpolacion-bilinear.jpg</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>159201</v>
+          <t>morfologicas\color</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>romboide-color-binaria.jpg</t>
+        </is>
       </c>
       <c r="C8" t="n">
-        <v>1596</v>
+        <v>33004</v>
+      </c>
+      <c r="D8" t="n">
+        <v>742</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>romboide-interpolacion-vecino.jpg</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>159201</v>
+          <t>morfologicas\color</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>romboide-color-contornos.jpg</t>
+        </is>
       </c>
       <c r="C9" t="n">
-        <v>1596</v>
+        <v>33004</v>
+      </c>
+      <c r="D9" t="n">
+        <v>742</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>romboide-multiplicacion.jpg</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>33004</v>
+          <t>morfologicas\color</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>romboide-color-figura-rellena.jpg</t>
+        </is>
       </c>
       <c r="C10" t="n">
+        <v>33004</v>
+      </c>
+      <c r="D10" t="n">
         <v>742</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>romboide-nitidez.jpg</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>32870</v>
+          <t>morfologicas\color</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>romboide-color-gris.jpg</t>
+        </is>
       </c>
       <c r="C11" t="n">
-        <v>844.4995617866516</v>
+        <v>33004</v>
+      </c>
+      <c r="D11" t="n">
+        <v>742</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>romboide-not1.jpg</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>8792.5</v>
+          <t>morfologicas\color</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>romboide-color-morfologica.jpg</t>
+        </is>
       </c>
       <c r="C12" t="n">
-        <v>420.634556889534</v>
+        <v>33004</v>
+      </c>
+      <c r="D12" t="n">
+        <v>742</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>romboide-not2.jpg</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>21497</v>
+          <t>morfologicas\sucio</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>romboide-sucio-binaria.jpg</t>
+        </is>
       </c>
       <c r="C13" t="n">
-        <v>618.9949476718903</v>
+        <v>33004</v>
+      </c>
+      <c r="D13" t="n">
+        <v>742</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>romboide-or.jpg</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>33004</v>
+          <t>morfologicas\sucio</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>romboide-sucio-contornos.jpg</t>
+        </is>
       </c>
       <c r="C14" t="n">
+        <v>33004</v>
+      </c>
+      <c r="D14" t="n">
         <v>742</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>romboide-redimensionada.jpg</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>159201</v>
+          <t>morfologicas\sucio</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>romboide-sucio-figura-rellena.jpg</t>
+        </is>
       </c>
       <c r="C15" t="n">
-        <v>1596</v>
+        <v>33004</v>
+      </c>
+      <c r="D15" t="n">
+        <v>742</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>romboide-resta.jpg</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0</v>
+          <t>morfologicas\sucio</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>romboide-sucio-gris.jpg</t>
+        </is>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>33004</v>
+      </c>
+      <c r="D16" t="n">
+        <v>742</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>romboide-rotado.jpg</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>8417.5</v>
+          <t>morfologicas\sucio</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>romboide-sucio-morfologica.jpg</t>
+        </is>
       </c>
       <c r="C17" t="n">
-        <v>491.771639585495</v>
+        <v>33004</v>
+      </c>
+      <c r="D17" t="n">
+        <v>742</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>romboide-suma.jpg</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>33004</v>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>romboide-and.jpg</t>
+        </is>
       </c>
       <c r="C18" t="n">
+        <v>33004</v>
+      </c>
+      <c r="D18" t="n">
         <v>742</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>romboide_bordes.jpg</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>8967.5</v>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>romboide-binarizado.jpg</t>
+        </is>
       </c>
       <c r="C19" t="n">
-        <v>411.3797236680984</v>
+        <v>33004</v>
+      </c>
+      <c r="D19" t="n">
+        <v>742</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>romboide_dilatado.jpg</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>33004</v>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>romboide-division.jpg</t>
+        </is>
       </c>
       <c r="C20" t="n">
-        <v>742</v>
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>romboide_Relieve.jpg</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>33001</v>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>romboide-gris.jpg</t>
+        </is>
       </c>
       <c r="C21" t="n">
-        <v>744.4852812290192</v>
+        <v>33004</v>
+      </c>
+      <c r="D21" t="n">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>romboide-interpolacion-bilinear.jpg</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>159201</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>romboide-interpolacion-vecino.jpg</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>159201</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>romboide-multiplicacion.jpg</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>33004</v>
+      </c>
+      <c r="D24" t="n">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>romboide-not1.jpg</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>8792.5</v>
+      </c>
+      <c r="D25" t="n">
+        <v>420.634556889534</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>romboide-not2.jpg</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>21497</v>
+      </c>
+      <c r="D26" t="n">
+        <v>618.9949476718903</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>romboide-or.jpg</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>33004</v>
+      </c>
+      <c r="D27" t="n">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>romboide-redimensionada.jpg</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>159201</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>romboide-resta.jpg</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>romboide-rotado.jpg</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>8417.5</v>
+      </c>
+      <c r="D30" t="n">
+        <v>491.771639585495</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Op</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>romboide-suma.jpg</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>33004</v>
+      </c>
+      <c r="D31" t="n">
+        <v>742</v>
       </c>
     </row>
   </sheetData>

</xml_diff>